<commit_message>
dernier push, formulaire d'avaluation du cours
</commit_message>
<xml_diff>
--- a/Excels_for_bg5/L1_DL.xlsx
+++ b/Excels_for_bg5/L1_DL.xlsx
@@ -615,8 +615,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -705,7 +705,7 @@
       </c>
       <c r="J2" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45999</v>
+        <v>46187</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>17</v>
@@ -750,7 +750,7 @@
       </c>
       <c r="J3" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42998</v>
+        <v>43175</v>
       </c>
       <c r="K3" s="0" t="s">
         <v>17</v>
@@ -795,7 +795,7 @@
       </c>
       <c r="J4" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43538</v>
+        <v>45773</v>
       </c>
       <c r="K4" s="0" t="s">
         <v>17</v>
@@ -840,7 +840,7 @@
       </c>
       <c r="J5" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45114</v>
+        <v>43855</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>17</v>
@@ -885,7 +885,7 @@
       </c>
       <c r="J6" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43597</v>
+        <v>45849</v>
       </c>
       <c r="K6" s="0" t="s">
         <v>17</v>
@@ -930,7 +930,7 @@
       </c>
       <c r="J7" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42828</v>
+        <v>45453</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>17</v>
@@ -975,7 +975,7 @@
       </c>
       <c r="J8" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45060</v>
+        <v>45467</v>
       </c>
       <c r="K8" s="0" t="s">
         <v>17</v>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="J9" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42466</v>
+        <v>45804</v>
       </c>
       <c r="K9" s="0" t="s">
         <v>17</v>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="J10" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44099</v>
+        <v>44012</v>
       </c>
       <c r="K10" s="0" t="s">
         <v>17</v>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="J11" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45042</v>
+        <v>44245</v>
       </c>
       <c r="K11" s="0" t="s">
         <v>17</v>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="J12" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43636</v>
+        <v>42814</v>
       </c>
       <c r="K12" s="0" t="s">
         <v>17</v>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="J13" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45540</v>
+        <v>45760</v>
       </c>
       <c r="K13" s="0" t="s">
         <v>17</v>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="J14" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42912</v>
+        <v>43187</v>
       </c>
       <c r="K14" s="0" t="s">
         <v>17</v>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="J15" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45795</v>
+        <v>43303</v>
       </c>
       <c r="K15" s="0" t="s">
         <v>17</v>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="J16" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42826</v>
+        <v>43696</v>
       </c>
       <c r="K16" s="0" t="s">
         <v>17</v>
@@ -1380,7 +1380,7 @@
       </c>
       <c r="J17" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45282</v>
+        <v>43003</v>
       </c>
       <c r="K17" s="0" t="s">
         <v>17</v>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="J18" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43659</v>
+        <v>46375</v>
       </c>
       <c r="K18" s="0" t="s">
         <v>17</v>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="J19" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44816</v>
+        <v>42508</v>
       </c>
       <c r="K19" s="0" t="s">
         <v>17</v>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="J20" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43066</v>
+        <v>42764</v>
       </c>
       <c r="K20" s="0" t="s">
         <v>17</v>
@@ -1560,7 +1560,7 @@
       </c>
       <c r="J21" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45783</v>
+        <v>43371</v>
       </c>
       <c r="K21" s="0" t="s">
         <v>17</v>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="J22" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43631</v>
+        <v>44315</v>
       </c>
       <c r="K22" s="0" t="s">
         <v>17</v>
@@ -1650,7 +1650,7 @@
       </c>
       <c r="J23" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43539</v>
+        <v>43398</v>
       </c>
       <c r="K23" s="0" t="s">
         <v>17</v>
@@ -1695,7 +1695,7 @@
       </c>
       <c r="J24" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42540</v>
+        <v>43884</v>
       </c>
       <c r="K24" s="0" t="s">
         <v>17</v>
@@ -1740,7 +1740,7 @@
       </c>
       <c r="J25" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42701</v>
+        <v>43912</v>
       </c>
       <c r="K25" s="0" t="s">
         <v>17</v>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="J26" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42901</v>
+        <v>46177</v>
       </c>
       <c r="K26" s="0" t="s">
         <v>17</v>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="J27" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44071</v>
+        <v>43909</v>
       </c>
       <c r="K27" s="0" t="s">
         <v>17</v>
@@ -1875,7 +1875,7 @@
       </c>
       <c r="J28" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44756</v>
+        <v>44754</v>
       </c>
       <c r="K28" s="0" t="s">
         <v>17</v>
@@ -1920,7 +1920,7 @@
       </c>
       <c r="J29" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44082</v>
+        <v>43845</v>
       </c>
       <c r="K29" s="0" t="s">
         <v>17</v>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="J30" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44562</v>
+        <v>45544</v>
       </c>
       <c r="K30" s="0" t="s">
         <v>17</v>
@@ -2010,7 +2010,7 @@
       </c>
       <c r="J31" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>46082</v>
+        <v>45125</v>
       </c>
       <c r="K31" s="0" t="s">
         <v>17</v>
@@ -2055,7 +2055,7 @@
       </c>
       <c r="J32" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44830</v>
+        <v>45712</v>
       </c>
       <c r="K32" s="0" t="s">
         <v>17</v>
@@ -2100,7 +2100,7 @@
       </c>
       <c r="J33" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44386</v>
+        <v>43270</v>
       </c>
       <c r="K33" s="0" t="s">
         <v>17</v>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="J34" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>46216</v>
+        <v>43613</v>
       </c>
       <c r="K34" s="0" t="s">
         <v>17</v>
@@ -2190,7 +2190,7 @@
       </c>
       <c r="J35" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42897</v>
+        <v>42454</v>
       </c>
       <c r="K35" s="0" t="s">
         <v>17</v>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="J36" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43276</v>
+        <v>43117</v>
       </c>
       <c r="K36" s="0" t="s">
         <v>17</v>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="J37" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>46364</v>
+        <v>45063</v>
       </c>
       <c r="K37" s="0" t="s">
         <v>17</v>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="J38" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>46230</v>
+        <v>45895</v>
       </c>
       <c r="K38" s="0" t="s">
         <v>17</v>
@@ -2370,7 +2370,7 @@
       </c>
       <c r="J39" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45386</v>
+        <v>43873</v>
       </c>
       <c r="K39" s="0" t="s">
         <v>17</v>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="J40" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44726</v>
+        <v>45733</v>
       </c>
       <c r="K40" s="0" t="s">
         <v>17</v>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="J41" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45145</v>
+        <v>43710</v>
       </c>
       <c r="K41" s="0" t="s">
         <v>17</v>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="J42" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42775</v>
+        <v>45048</v>
       </c>
       <c r="K42" s="0" t="s">
         <v>17</v>
@@ -2550,7 +2550,7 @@
       </c>
       <c r="J43" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45875</v>
+        <v>43772</v>
       </c>
       <c r="K43" s="0" t="s">
         <v>17</v>
@@ -2595,7 +2595,7 @@
       </c>
       <c r="J44" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43470</v>
+        <v>43711</v>
       </c>
       <c r="K44" s="0" t="s">
         <v>17</v>
@@ -2640,7 +2640,7 @@
       </c>
       <c r="J45" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44899</v>
+        <v>46118</v>
       </c>
       <c r="K45" s="0" t="s">
         <v>17</v>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="J46" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44751</v>
+        <v>46303</v>
       </c>
       <c r="K46" s="0" t="s">
         <v>17</v>
@@ -2730,7 +2730,7 @@
       </c>
       <c r="J47" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>46305</v>
+        <v>45642</v>
       </c>
       <c r="K47" s="0" t="s">
         <v>17</v>
@@ -2775,7 +2775,7 @@
       </c>
       <c r="J48" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43210</v>
+        <v>45170</v>
       </c>
       <c r="K48" s="0" t="s">
         <v>17</v>
@@ -2820,7 +2820,7 @@
       </c>
       <c r="J49" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42788</v>
+        <v>43382</v>
       </c>
       <c r="K49" s="0" t="s">
         <v>17</v>
@@ -2865,7 +2865,7 @@
       </c>
       <c r="J50" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44048</v>
+        <v>44504</v>
       </c>
       <c r="K50" s="0" t="s">
         <v>17</v>
@@ -2910,7 +2910,7 @@
       </c>
       <c r="J51" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45170</v>
+        <v>44933</v>
       </c>
       <c r="K51" s="0" t="s">
         <v>17</v>
@@ -2955,7 +2955,7 @@
       </c>
       <c r="J52" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45558</v>
+        <v>45495</v>
       </c>
       <c r="K52" s="0" t="s">
         <v>17</v>
@@ -3000,7 +3000,7 @@
       </c>
       <c r="J53" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42639</v>
+        <v>44067</v>
       </c>
       <c r="K53" s="0" t="s">
         <v>17</v>
@@ -3045,7 +3045,7 @@
       </c>
       <c r="J54" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42654</v>
+        <v>46324</v>
       </c>
       <c r="K54" s="0" t="s">
         <v>17</v>
@@ -3090,7 +3090,7 @@
       </c>
       <c r="J55" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45017</v>
+        <v>42460</v>
       </c>
       <c r="K55" s="0" t="s">
         <v>17</v>
@@ -3135,7 +3135,7 @@
       </c>
       <c r="J56" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42751</v>
+        <v>44809</v>
       </c>
       <c r="K56" s="0" t="s">
         <v>17</v>
@@ -3180,7 +3180,7 @@
       </c>
       <c r="J57" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45634</v>
+        <v>45917</v>
       </c>
       <c r="K57" s="0" t="s">
         <v>17</v>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="J58" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43560</v>
+        <v>44659</v>
       </c>
       <c r="K58" s="0" t="s">
         <v>17</v>
@@ -3270,7 +3270,7 @@
       </c>
       <c r="J59" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>45739</v>
+        <v>45573</v>
       </c>
       <c r="K59" s="0" t="s">
         <v>17</v>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="J60" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42634</v>
+        <v>45779</v>
       </c>
       <c r="K60" s="0" t="s">
         <v>17</v>
@@ -3360,7 +3360,7 @@
       </c>
       <c r="J61" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43215</v>
+        <v>42734</v>
       </c>
       <c r="K61" s="0" t="s">
         <v>17</v>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="J62" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43829</v>
+        <v>42879</v>
       </c>
       <c r="K62" s="0" t="s">
         <v>17</v>
@@ -3450,7 +3450,7 @@
       </c>
       <c r="J63" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44319</v>
+        <v>43900</v>
       </c>
       <c r="K63" s="0" t="s">
         <v>17</v>
@@ -3495,7 +3495,7 @@
       </c>
       <c r="J64" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>46313</v>
+        <v>45735</v>
       </c>
       <c r="K64" s="0" t="s">
         <v>17</v>
@@ -3540,7 +3540,7 @@
       </c>
       <c r="J65" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43582</v>
+        <v>44363</v>
       </c>
       <c r="K65" s="0" t="s">
         <v>17</v>
@@ -3585,7 +3585,7 @@
       </c>
       <c r="J66" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44473</v>
+        <v>42796</v>
       </c>
       <c r="K66" s="0" t="s">
         <v>17</v>
@@ -3630,7 +3630,7 @@
       </c>
       <c r="J67" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44230</v>
+        <v>44224</v>
       </c>
       <c r="K67" s="0" t="s">
         <v>17</v>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="J68" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42788</v>
+        <v>44794</v>
       </c>
       <c r="K68" s="0" t="s">
         <v>17</v>
@@ -3720,7 +3720,7 @@
       </c>
       <c r="J69" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44143</v>
+        <v>45506</v>
       </c>
       <c r="K69" s="0" t="s">
         <v>17</v>
@@ -3765,7 +3765,7 @@
       </c>
       <c r="J70" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44691</v>
+        <v>45882</v>
       </c>
       <c r="K70" s="0" t="s">
         <v>17</v>
@@ -3810,7 +3810,7 @@
       </c>
       <c r="J71" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>42541</v>
+        <v>44642</v>
       </c>
       <c r="K71" s="0" t="s">
         <v>17</v>
@@ -3855,7 +3855,7 @@
       </c>
       <c r="J72" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>46333</v>
+        <v>45606</v>
       </c>
       <c r="K72" s="0" t="s">
         <v>17</v>
@@ -3900,7 +3900,7 @@
       </c>
       <c r="J73" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43884</v>
+        <v>42569</v>
       </c>
       <c r="K73" s="0" t="s">
         <v>17</v>
@@ -3945,7 +3945,7 @@
       </c>
       <c r="J74" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>43336</v>
+        <v>43606</v>
       </c>
       <c r="K74" s="0" t="s">
         <v>17</v>
@@ -3990,7 +3990,7 @@
       </c>
       <c r="J75" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>46385</v>
+        <v>42513</v>
       </c>
       <c r="K75" s="0" t="s">
         <v>17</v>
@@ -4035,7 +4035,7 @@
       </c>
       <c r="J76" s="2" t="n">
         <f aca="true">com.sun.star.sheet.addin.Analysis.getRandbetween(TODAY()-3000,TODAY()+1000)</f>
-        <v>44571</v>
+        <v>42804</v>
       </c>
       <c r="K76" s="0" t="s">
         <v>17</v>

</xml_diff>